<commit_message>
Logs and data from new set of experiments
</commit_message>
<xml_diff>
--- a/evaluation/data/plot.xlsx
+++ b/evaluation/data/plot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/dev/cl/move-op/evaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDBBF62-84A7-E249-B137-704FEAFCB731}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825C7E1E-7AAF-4B44-891D-A26F9F06FBC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36180" yWindow="-3720" windowWidth="22380" windowHeight="21600" xr2:uid="{0A30AF39-E39C-7545-8255-958495C45241}"/>
+    <workbookView xWindow="30420" yWindow="-3720" windowWidth="22380" windowHeight="21600" xr2:uid="{0A30AF39-E39C-7545-8255-958495C45241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t>us-west-1</t>
   </si>
@@ -74,14 +74,14 @@
   <si>
     <t>pos-error</t>
   </si>
-  <si>
-    <t>repeated:</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -111,10 +111,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,7 +136,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -151,8 +152,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8849856279701573E-2"/>
-          <c:y val="4.7219117953250414E-2"/>
+          <c:x val="7.5447446662528186E-2"/>
+          <c:y val="5.0822728240051074E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -168,7 +169,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -224,48 +225,66 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$AA$4:$AA$8</c:f>
+                <c:f>Sheet1!$AA$4:$AA$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.51666666666666672</c:v>
+                    <c:v>7.3333333333333334E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.6433333333333332</c:v>
+                    <c:v>0.11000000000000001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.4833333333333336</c:v>
+                    <c:v>0.23333333333333334</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.4033333333333342</c:v>
+                    <c:v>0.21000000000000008</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.0833333333333339</c:v>
+                    <c:v>0.14666666666666672</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.3566666666666668</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.9700000000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.82000000000000006</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$Y$4:$Y$8</c:f>
+                <c:f>Sheet1!$Y$4:$Y$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.13</c:v>
+                    <c:v>0.11333333333333334</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.45000000000000012</c:v>
+                    <c:v>0.11666666666666667</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0166666666666666</c:v>
+                    <c:v>0.17333333333333337</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.7100000000000002</c:v>
+                    <c:v>0.24999999999999997</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.8433333333333333</c:v>
+                    <c:v>0.26999999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.36999999999999988</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.5299999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.1500000000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -286,66 +305,72 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$4:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.964071856287426</c:v>
+                  <c:v>214.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>299.96999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.641025641025642</c:v>
+                  <c:v>428.53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.027027027027028</c:v>
+                  <c:v>499.93</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>599.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>602.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$4:$Z$11</c:f>
+              <c:f>Sheet1!$Z$4:$Z$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.21333333333333335</c:v>
+                  <c:v>0.14333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56666666666666676</c:v>
+                  <c:v>0.17666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2033333333333334</c:v>
+                  <c:v>0.35000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0233333333333334</c:v>
+                  <c:v>0.43999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3466666666666667</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.153333333333336</c:v>
+                  <c:v>0.8933333333333332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.49666666666667</c:v>
+                  <c:v>1.0233333333333332</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.546666666666667</c:v>
+                  <c:v>1.3433333333333335</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4933333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -372,7 +397,8 @@
         <c:axId val="1863051663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30"/>
+          <c:max val="610"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -435,7 +461,8 @@
         <c:axId val="1865321615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12"/>
+          <c:max val="2.4"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -500,7 +527,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
-        <c:minorUnit val="1"/>
+        <c:minorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -529,7 +556,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -545,8 +572,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8304637546707831E-2"/>
-          <c:y val="0.11500609635803248"/>
+          <c:x val="8.8979437386277629E-2"/>
+          <c:y val="0.10210354350655657"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -562,7 +589,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -618,66 +645,72 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$X$4:$X$11</c:f>
+                <c:f>Sheet1!$X$4:$X$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
+                  <c:ptCount val="11"/>
                   <c:pt idx="0">
-                    <c:v>1.3900000000000001</c:v>
+                    <c:v>2.6666666666666658E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.5633333333333332</c:v>
+                    <c:v>2.6666666666666665E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.3899999999999997</c:v>
+                    <c:v>1.6666666666666677E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.51000000000000012</c:v>
+                    <c:v>1.666666666666667E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.92666666666666675</c:v>
+                    <c:v>1.6666666666666656E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.80333333333333323</c:v>
+                    <c:v>1.0000000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.94666666666666677</c:v>
+                    <c:v>1.3333333333333329E-2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>1.0533333333333335</c:v>
+                    <c:v>1.3333333333333329E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.3333333333333329E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$V$4:$V$11</c:f>
+                <c:f>Sheet1!$V$4:$V$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
+                  <c:ptCount val="11"/>
                   <c:pt idx="0">
-                    <c:v>0.10666666666666665</c:v>
+                    <c:v>5.6666666666666671E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.20333333333333337</c:v>
+                    <c:v>4.3333333333333328E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.55999999999999994</c:v>
+                    <c:v>4.9999999999999996E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.35666666666666663</c:v>
+                    <c:v>4.3333333333333335E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.33999999999999997</c:v>
+                    <c:v>4.0000000000000008E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.83000000000000007</c:v>
+                    <c:v>4.3333333333333335E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.36</c:v>
+                    <c:v>4.3333333333333335E-2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.37</c:v>
+                    <c:v>4.3333333333333335E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.3333333333333342E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -698,66 +731,72 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$4:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.964071856287426</c:v>
+                  <c:v>214.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>299.96999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.641025641025642</c:v>
+                  <c:v>428.53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.027027027027028</c:v>
+                  <c:v>499.93</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>599.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>602.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$4:$W$11</c:f>
+              <c:f>Sheet1!$W$4:$W$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19666666666666666</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27</c:v>
+                  <c:v>5.6666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62666666666666659</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39333333333333331</c:v>
+                  <c:v>5.3333333333333337E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38999999999999996</c:v>
+                  <c:v>5.000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8666666666666667</c:v>
+                  <c:v>5.3333333333333337E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.38999999999999996</c:v>
+                  <c:v>5.3333333333333337E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41333333333333333</c:v>
+                  <c:v>5.3333333333333337E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,7 +823,8 @@
         <c:axId val="1863051663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30"/>
+          <c:max val="610"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -809,10 +849,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" baseline="0"/>
+                  <a:defRPr sz="1800" b="0" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1800" b="0" baseline="0"/>
                   <a:t>Move operations per second</a:t>
                 </a:r>
               </a:p>
@@ -865,7 +905,7 @@
         <c:axId val="1865321615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3"/>
+          <c:max val="0.1"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -893,7 +933,7 @@
             </a:ln>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -933,8 +973,7 @@
         <c:crossAx val="1863051663"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-        <c:minorUnit val="1"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -965,15 +1004,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1001,15 +1040,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>120651</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1336,9 +1375,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FD8EE4-C80E-7B4A-A3CF-4A016730C7B3}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1491,795 +1532,794 @@
       </c>
     </row>
     <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B4" s="2">
-        <f>3*1000/A4</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.09</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>0.17</v>
+      </c>
+      <c r="H4">
+        <v>0.25</v>
+      </c>
+      <c r="I4">
+        <v>0.02</v>
+      </c>
+      <c r="J4">
+        <v>0.08</v>
+      </c>
+      <c r="K4">
+        <v>0.12</v>
+      </c>
+      <c r="L4">
+        <v>0.01</v>
+      </c>
+      <c r="M4">
+        <v>0.1</v>
+      </c>
+      <c r="N4">
+        <v>0.17</v>
+      </c>
+      <c r="O4">
+        <v>0.01</v>
+      </c>
+      <c r="P4">
         <v>0.06</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.61</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="Q4">
         <v>0.08</v>
       </c>
-      <c r="J4" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.99</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>2.16</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="T4" s="1">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="V4" s="1">
+      <c r="R4">
+        <v>0.06</v>
+      </c>
+      <c r="S4">
+        <v>0.16</v>
+      </c>
+      <c r="T4">
+        <v>0.23</v>
+      </c>
+      <c r="V4" s="3">
         <f>W4-AVERAGE(C4,I4,O4)</f>
-        <v>0.10666666666666665</v>
-      </c>
-      <c r="W4" s="1">
+        <v>5.6666666666666671E-2</v>
+      </c>
+      <c r="W4" s="3">
         <f t="shared" ref="W4:Z4" si="0">AVERAGE(D4,J4,P4)</f>
-        <v>0.19666666666666666</v>
-      </c>
-      <c r="X4" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X4" s="3">
         <f>AVERAGE(E4,K4,Q4)-W4</f>
-        <v>1.3900000000000001</v>
-      </c>
-      <c r="Y4" s="1">
+        <v>2.6666666666666658E-2</v>
+      </c>
+      <c r="Y4" s="3">
         <f>Z4-AVERAGE(F4,L4,R4)</f>
-        <v>0.13</v>
-      </c>
-      <c r="Z4" s="1">
+        <v>0.11333333333333334</v>
+      </c>
+      <c r="Z4" s="3">
         <f t="shared" si="0"/>
-        <v>0.21333333333333335</v>
-      </c>
-      <c r="AA4" s="1">
+        <v>0.14333333333333334</v>
+      </c>
+      <c r="AA4" s="3">
         <f>AVERAGE(H4,N4,T4)-Z4</f>
-        <v>0.51666666666666672</v>
+        <v>7.3333333333333334E-2</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>500</v>
-      </c>
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B8" si="1">3*1000/A5</f>
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>0.01</v>
+      </c>
+      <c r="D5">
+        <v>0.06</v>
+      </c>
+      <c r="E5">
+        <v>0.09</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
+        <v>0.17</v>
+      </c>
+      <c r="H5">
         <v>0.25</v>
       </c>
-      <c r="E5" s="1">
-        <v>1.78</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1.24</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1.82</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1.65</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="I5">
+        <v>0.02</v>
+      </c>
+      <c r="J5">
+        <v>0.06</v>
+      </c>
+      <c r="K5">
+        <v>0.09</v>
+      </c>
+      <c r="L5">
+        <v>0.01</v>
+      </c>
+      <c r="M5">
+        <v>0.11</v>
+      </c>
+      <c r="N5">
+        <v>0.32</v>
+      </c>
+      <c r="O5">
+        <v>0.01</v>
+      </c>
+      <c r="P5">
+        <v>0.05</v>
+      </c>
+      <c r="Q5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S5" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0.74</v>
-      </c>
-      <c r="V5" s="1">
-        <f t="shared" ref="V5:V8" si="2">W5-AVERAGE(C5,I5,O5)</f>
-        <v>0.20333333333333337</v>
-      </c>
-      <c r="W5" s="1">
-        <f t="shared" ref="W5:W8" si="3">AVERAGE(D5,J5,P5)</f>
-        <v>0.27</v>
-      </c>
-      <c r="X5" s="1">
-        <f t="shared" ref="X5:X8" si="4">AVERAGE(E5,K5,Q5)-W5</f>
-        <v>1.5633333333333332</v>
-      </c>
-      <c r="Y5" s="1">
-        <f t="shared" ref="Y5:Y8" si="5">Z5-AVERAGE(F5,L5,R5)</f>
-        <v>0.45000000000000012</v>
-      </c>
-      <c r="Z5" s="1">
-        <f t="shared" ref="Z5:Z8" si="6">AVERAGE(G5,M5,S5)</f>
-        <v>0.56666666666666676</v>
-      </c>
-      <c r="AA5" s="1">
-        <f t="shared" ref="AA5:AA8" si="7">AVERAGE(H5,N5,T5)-Z5</f>
-        <v>0.6433333333333332</v>
+      <c r="R5">
+        <v>0.12</v>
+      </c>
+      <c r="S5">
+        <v>0.25</v>
+      </c>
+      <c r="T5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" ref="V5:V11" si="1">W5-AVERAGE(C5,I5,O5)</f>
+        <v>4.3333333333333328E-2</v>
+      </c>
+      <c r="W5" s="3">
+        <f t="shared" ref="W5:W11" si="2">AVERAGE(D5,J5,P5)</f>
+        <v>5.6666666666666664E-2</v>
+      </c>
+      <c r="X5" s="3">
+        <f t="shared" ref="X5:X11" si="3">AVERAGE(E5,K5,Q5)-W5</f>
+        <v>2.6666666666666665E-2</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" ref="Y5:Y11" si="4">Z5-AVERAGE(F5,L5,R5)</f>
+        <v>0.11666666666666667</v>
+      </c>
+      <c r="Z5" s="3">
+        <f t="shared" ref="Z5:Z11" si="5">AVERAGE(G5,M5,S5)</f>
+        <v>0.17666666666666667</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" ref="AA5:AA11" si="6">AVERAGE(H5,N5,T5)-Z5</f>
+        <v>0.11000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>250</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>0.06</v>
+      </c>
+      <c r="E6">
+        <v>0.08</v>
+      </c>
+      <c r="F6">
+        <v>0.05</v>
+      </c>
+      <c r="G6">
+        <v>0.23</v>
+      </c>
+      <c r="H6">
+        <v>0.37</v>
+      </c>
+      <c r="I6">
+        <v>0.01</v>
+      </c>
+      <c r="J6">
+        <v>0.06</v>
+      </c>
+      <c r="K6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.1</v>
+      </c>
+      <c r="M6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N6">
+        <v>0.66</v>
+      </c>
+      <c r="O6">
+        <v>0.01</v>
+      </c>
+      <c r="P6">
+        <v>0.06</v>
+      </c>
+      <c r="Q6">
+        <v>0.08</v>
+      </c>
+      <c r="R6">
+        <v>0.38</v>
+      </c>
+      <c r="S6">
+        <v>0.54</v>
+      </c>
+      <c r="T6">
+        <v>0.72</v>
+      </c>
+      <c r="V6" s="3">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.41</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1.83</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1.49</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3.01</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="K6" s="1">
-        <v>2.19</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <v>2.62</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="S6" s="1">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="T6" s="1">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="V6" s="1">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="W6" s="3">
         <f t="shared" si="2"/>
-        <v>0.55999999999999994</v>
-      </c>
-      <c r="W6" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="X6" s="3">
         <f t="shared" si="3"/>
-        <v>0.62666666666666659</v>
-      </c>
-      <c r="X6" s="1">
+        <v>1.6666666666666677E-2</v>
+      </c>
+      <c r="Y6" s="3">
         <f t="shared" si="4"/>
-        <v>1.3899999999999997</v>
-      </c>
-      <c r="Y6" s="1">
+        <v>0.17333333333333337</v>
+      </c>
+      <c r="Z6" s="3">
         <f t="shared" si="5"/>
-        <v>1.0166666666666666</v>
-      </c>
-      <c r="Z6" s="1">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="AA6" s="3">
         <f t="shared" si="6"/>
-        <v>1.2033333333333334</v>
-      </c>
-      <c r="AA6" s="1">
-        <f t="shared" si="7"/>
-        <v>1.4833333333333336</v>
+        <v>0.23333333333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>167</v>
-      </c>
-      <c r="B7" s="2">
-        <f t="shared" si="1"/>
-        <v>17.964071856287426</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.34</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2.54</v>
-      </c>
-      <c r="H7" s="1">
-        <v>13.6</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1.48</v>
-      </c>
-      <c r="L7" s="1">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>214.29</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>0.06</v>
+      </c>
+      <c r="E7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F7">
         <v>0.05</v>
       </c>
-      <c r="M7" s="1">
-        <v>2.21</v>
-      </c>
-      <c r="N7" s="1">
-        <v>8.43</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0.41</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="S7" s="1">
-        <v>1.32</v>
-      </c>
-      <c r="T7" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="V7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.35666666666666663</v>
-      </c>
-      <c r="W7" s="1">
-        <f t="shared" si="3"/>
-        <v>0.39333333333333331</v>
-      </c>
-      <c r="X7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.51000000000000012</v>
-      </c>
-      <c r="Y7" s="1">
-        <f t="shared" si="5"/>
-        <v>1.7100000000000002</v>
-      </c>
-      <c r="Z7" s="1">
-        <f t="shared" si="6"/>
-        <v>2.0233333333333334</v>
-      </c>
-      <c r="AA7" s="1">
-        <f t="shared" si="7"/>
-        <v>6.4033333333333342</v>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <v>0.59</v>
+      </c>
+      <c r="I7">
+        <v>0.01</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+      <c r="K7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.05</v>
+      </c>
+      <c r="M7">
+        <v>0.36</v>
+      </c>
+      <c r="N7">
+        <v>0.61</v>
+      </c>
+      <c r="O7">
+        <v>0.01</v>
+      </c>
+      <c r="P7">
+        <v>0.05</v>
+      </c>
+      <c r="Q7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R7">
+        <v>0.47</v>
+      </c>
+      <c r="S7">
+        <v>0.66</v>
+      </c>
+      <c r="T7">
+        <v>0.75</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" ref="V7" si="7">W7-AVERAGE(C7,I7,O7)</f>
+        <v>4.3333333333333335E-2</v>
+      </c>
+      <c r="W7" s="3">
+        <f t="shared" ref="W7" si="8">AVERAGE(D7,J7,P7)</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="X7" s="3">
+        <f t="shared" ref="X7" si="9">AVERAGE(E7,K7,Q7)-W7</f>
+        <v>1.666666666666667E-2</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" ref="Y7" si="10">Z7-AVERAGE(F7,L7,R7)</f>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="Z7" s="3">
+        <f t="shared" ref="Z7" si="11">AVERAGE(G7,M7,S7)</f>
+        <v>0.43999999999999995</v>
+      </c>
+      <c r="AA7" s="3">
+        <f t="shared" ref="AA7" si="12">AVERAGE(H7,N7,T7)-Z7</f>
+        <v>0.21000000000000008</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>125</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>299.96999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.01</v>
+      </c>
+      <c r="D8">
+        <v>0.05</v>
+      </c>
+      <c r="E8">
+        <v>0.06</v>
+      </c>
+      <c r="F8">
+        <v>0.15</v>
+      </c>
+      <c r="G8">
+        <v>0.51</v>
+      </c>
+      <c r="H8">
+        <v>0.74</v>
+      </c>
+      <c r="I8">
+        <v>0.01</v>
+      </c>
+      <c r="J8">
+        <v>0.05</v>
+      </c>
+      <c r="K8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M8">
+        <v>0.45</v>
+      </c>
+      <c r="N8">
+        <v>0.52</v>
+      </c>
+      <c r="O8">
+        <v>0.01</v>
+      </c>
+      <c r="P8">
+        <v>0.05</v>
+      </c>
+      <c r="Q8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R8">
+        <v>0.59</v>
+      </c>
+      <c r="S8">
+        <v>0.87</v>
+      </c>
+      <c r="T8">
+        <v>1.01</v>
+      </c>
+      <c r="V8" s="3">
         <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="C8" s="1">
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="W8" s="3">
+        <f t="shared" si="2"/>
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="X8" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666656E-2</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="4"/>
+        <v>0.26999999999999996</v>
+      </c>
+      <c r="Z8" s="3">
+        <f t="shared" si="5"/>
+        <v>0.61</v>
+      </c>
+      <c r="AA8" s="3">
+        <f t="shared" si="6"/>
+        <v>0.14666666666666672</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>428.53</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.06</v>
+      </c>
+      <c r="E9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1.42</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="H8" s="1">
-        <v>4.18</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.81</v>
-      </c>
-      <c r="L8" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="N8" s="1">
-        <v>4.96</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>1.72</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="S8" s="1">
-        <v>2.08</v>
-      </c>
-      <c r="T8" s="1">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="V8" s="1">
+      <c r="F9">
+        <v>0.34</v>
+      </c>
+      <c r="G9">
+        <v>0.95</v>
+      </c>
+      <c r="H9">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I9">
+        <v>0.01</v>
+      </c>
+      <c r="J9">
+        <v>0.05</v>
+      </c>
+      <c r="K9">
+        <v>0.06</v>
+      </c>
+      <c r="L9">
+        <v>0.13</v>
+      </c>
+      <c r="M9">
+        <v>0.45</v>
+      </c>
+      <c r="N9">
+        <v>1.2</v>
+      </c>
+      <c r="O9">
+        <v>0.01</v>
+      </c>
+      <c r="P9">
+        <v>0.05</v>
+      </c>
+      <c r="Q9">
+        <v>0.06</v>
+      </c>
+      <c r="R9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S9">
+        <v>1.28</v>
+      </c>
+      <c r="T9">
+        <v>1.41</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333335E-2</v>
+      </c>
+      <c r="W9" s="3">
         <f t="shared" si="2"/>
-        <v>0.33999999999999997</v>
-      </c>
-      <c r="W8" s="1">
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="X9" s="3">
         <f t="shared" si="3"/>
-        <v>0.38999999999999996</v>
-      </c>
-      <c r="X8" s="1">
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="Y9" s="3">
         <f t="shared" si="4"/>
-        <v>0.92666666666666675</v>
-      </c>
-      <c r="Y8" s="1">
+        <v>0.36999999999999988</v>
+      </c>
+      <c r="Z9" s="3">
         <f t="shared" si="5"/>
-        <v>1.8433333333333333</v>
-      </c>
-      <c r="Z8" s="1">
+        <v>0.8933333333333332</v>
+      </c>
+      <c r="AA9" s="3">
         <f t="shared" si="6"/>
-        <v>2.3466666666666667</v>
-      </c>
-      <c r="AA8" s="1">
-        <f t="shared" si="7"/>
-        <v>2.0833333333333339</v>
+        <v>0.3566666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>117</v>
-      </c>
-      <c r="B9" s="2">
-        <f>3*1000/A9</f>
-        <v>25.641025641025642</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1.51</v>
-      </c>
-      <c r="F9" s="1">
-        <v>3.72</v>
-      </c>
-      <c r="G9" s="1">
-        <v>27.63</v>
-      </c>
-      <c r="H9" s="1">
-        <v>76.89</v>
-      </c>
-      <c r="I9" s="1">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>499.93</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+      <c r="D10">
         <v>0.05</v>
       </c>
-      <c r="J9" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1.68</v>
-      </c>
-      <c r="L9" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="M9" s="1">
-        <v>29.3</v>
-      </c>
-      <c r="N9" s="1">
-        <v>102</v>
-      </c>
-      <c r="O9" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="P9" s="1">
-        <v>1.07</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>1.82</v>
-      </c>
-      <c r="R9" s="1">
-        <v>3.37</v>
-      </c>
-      <c r="S9" s="1">
-        <v>30.53</v>
-      </c>
-      <c r="T9" s="1">
-        <v>96.04</v>
-      </c>
-      <c r="V9" s="1">
-        <f>W9-AVERAGE(C9,I9,O9)</f>
-        <v>0.83000000000000007</v>
-      </c>
-      <c r="W9" s="1">
-        <f>AVERAGE(D9,J9,P9)</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="X9" s="1">
-        <f>AVERAGE(E9,K9,Q9)-W9</f>
-        <v>0.80333333333333323</v>
-      </c>
-      <c r="Y9" s="1">
-        <f>Z9-AVERAGE(F9,L9,R9)</f>
-        <v>26.206666666666671</v>
-      </c>
-      <c r="Z9" s="1">
-        <f>AVERAGE(G9,M9,S9)</f>
-        <v>29.153333333333336</v>
-      </c>
-      <c r="AA9" s="1">
-        <f>AVERAGE(H9,N9,T9)-Z9</f>
-        <v>62.489999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>111</v>
-      </c>
-      <c r="B10" s="2">
-        <f>3*1000/A10</f>
-        <v>27.027027027027028</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="G10" s="1">
-        <v>33.49</v>
-      </c>
-      <c r="H10" s="1">
-        <v>81.28</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1.36</v>
-      </c>
-      <c r="L10" s="1">
-        <v>4.78</v>
-      </c>
-      <c r="M10" s="1">
-        <v>35.130000000000003</v>
-      </c>
-      <c r="N10" s="1">
-        <v>85.04</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="R10" s="1">
-        <v>7.49</v>
-      </c>
-      <c r="S10" s="1">
-        <v>40.869999999999997</v>
-      </c>
-      <c r="T10" s="1">
-        <v>90.98</v>
-      </c>
-      <c r="V10" s="1">
-        <f>W10-AVERAGE(C10,I10,O10)</f>
-        <v>0.36</v>
-      </c>
-      <c r="W10" s="1">
-        <f>AVERAGE(D10,J10,P10)</f>
-        <v>0.38999999999999996</v>
-      </c>
-      <c r="X10" s="1">
-        <f>AVERAGE(E10,K10,Q10)-W10</f>
-        <v>0.94666666666666677</v>
-      </c>
-      <c r="Y10" s="1">
-        <f>Z10-AVERAGE(F10,L10,R10)</f>
-        <v>32.123333333333335</v>
-      </c>
-      <c r="Z10" s="1">
-        <f>AVERAGE(G10,M10,S10)</f>
-        <v>36.49666666666667</v>
-      </c>
-      <c r="AA10" s="1">
-        <f>AVERAGE(H10,N10,T10)-Z10</f>
-        <v>49.269999999999996</v>
+      <c r="E10">
+        <v>0.06</v>
+      </c>
+      <c r="F10">
+        <v>0.82</v>
+      </c>
+      <c r="G10">
+        <v>1.46</v>
+      </c>
+      <c r="H10">
+        <v>2.23</v>
+      </c>
+      <c r="I10">
+        <v>0.01</v>
+      </c>
+      <c r="J10">
+        <v>0.06</v>
+      </c>
+      <c r="K10">
+        <v>0.08</v>
+      </c>
+      <c r="L10">
+        <v>0.37</v>
+      </c>
+      <c r="M10">
+        <v>0.79</v>
+      </c>
+      <c r="N10">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="O10">
+        <v>0.01</v>
+      </c>
+      <c r="P10">
+        <v>0.05</v>
+      </c>
+      <c r="Q10">
+        <v>0.06</v>
+      </c>
+      <c r="R10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S10">
+        <v>0.82</v>
+      </c>
+      <c r="T10">
+        <v>1.49</v>
+      </c>
+      <c r="V10" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333335E-2</v>
+      </c>
+      <c r="W10" s="3">
+        <f t="shared" si="2"/>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="X10" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333329E-2</v>
+      </c>
+      <c r="Y10" s="3">
+        <f t="shared" si="4"/>
+        <v>0.5299999999999998</v>
+      </c>
+      <c r="Z10" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0233333333333332</v>
+      </c>
+      <c r="AA10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.9700000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>100</v>
-      </c>
-      <c r="B11" s="2">
-        <f>3*1000/A11</f>
-        <v>30</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>599.96</v>
+      </c>
+      <c r="C11">
+        <v>0.01</v>
+      </c>
+      <c r="D11">
+        <v>0.05</v>
+      </c>
+      <c r="E11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.22</v>
+      </c>
+      <c r="G11">
+        <v>1.25</v>
+      </c>
+      <c r="H11">
+        <v>2.42</v>
+      </c>
+      <c r="I11">
+        <v>0.01</v>
+      </c>
+      <c r="J11">
+        <v>0.06</v>
+      </c>
+      <c r="K11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L11">
+        <v>0.31</v>
+      </c>
+      <c r="M11">
+        <v>1.53</v>
+      </c>
+      <c r="N11">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="O11">
+        <v>0.01</v>
+      </c>
+      <c r="P11">
+        <v>0.05</v>
+      </c>
+      <c r="Q11">
+        <v>0.06</v>
+      </c>
+      <c r="R11">
+        <v>0.05</v>
+      </c>
+      <c r="S11">
+        <v>1.25</v>
+      </c>
+      <c r="T11">
+        <v>1.56</v>
+      </c>
+      <c r="V11" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333335E-2</v>
+      </c>
+      <c r="W11" s="3">
+        <f t="shared" si="2"/>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="X11" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333329E-2</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="4"/>
+        <v>1.1500000000000001</v>
+      </c>
+      <c r="Z11" s="3">
+        <f t="shared" si="5"/>
+        <v>1.3433333333333335</v>
+      </c>
+      <c r="AA11" s="3">
+        <f t="shared" si="6"/>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>602.03</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.05</v>
+      </c>
+      <c r="E12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.01</v>
+      </c>
+      <c r="G12">
+        <v>1.59</v>
+      </c>
+      <c r="H12">
+        <v>3.67</v>
+      </c>
+      <c r="I12">
+        <v>0.01</v>
+      </c>
+      <c r="J12">
+        <v>0.05</v>
+      </c>
+      <c r="K12">
+        <v>0.06</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1.45</v>
+      </c>
+      <c r="N12">
+        <v>3.56</v>
+      </c>
+      <c r="O12">
+        <v>0.01</v>
+      </c>
+      <c r="P12">
+        <v>0.05</v>
+      </c>
+      <c r="Q12">
+        <v>0.06</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1.44</v>
+      </c>
+      <c r="T12">
+        <v>3.69</v>
+      </c>
+      <c r="V12" s="3">
+        <f>W12-AVERAGE(C12,I12,O12)</f>
+        <v>4.3333333333333342E-2</v>
+      </c>
+      <c r="W12" s="3">
+        <f>AVERAGE(D12,J12,P12)</f>
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="X12" s="3">
+        <f>AVERAGE(E12,K12,Q12)-W12</f>
+        <v>1.3333333333333329E-2</v>
+      </c>
+      <c r="Y12" s="3">
+        <f>Z12-AVERAGE(F12,L12,R12)</f>
         <v>1.49</v>
       </c>
-      <c r="F11" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>37.81</v>
-      </c>
-      <c r="H11" s="1">
-        <v>90.06</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1.58</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0.36</v>
-      </c>
-      <c r="M11" s="1">
-        <v>42.75</v>
-      </c>
-      <c r="N11" s="1">
-        <v>94.83</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.36</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>1.33</v>
-      </c>
-      <c r="R11" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="S11" s="1">
-        <v>35.08</v>
-      </c>
-      <c r="T11" s="1">
-        <v>101.32</v>
-      </c>
-      <c r="V11" s="1">
-        <f>W11-AVERAGE(C11,I11,O11)</f>
-        <v>0.37</v>
-      </c>
-      <c r="W11" s="1">
-        <f>AVERAGE(D11,J11,P11)</f>
-        <v>0.41333333333333333</v>
-      </c>
-      <c r="X11" s="1">
-        <f>AVERAGE(E11,K11,Q11)-W11</f>
-        <v>1.0533333333333335</v>
-      </c>
-      <c r="Y11" s="1">
-        <f>Z11-AVERAGE(F11,L11,R11)</f>
-        <v>37.973333333333336</v>
-      </c>
-      <c r="Z11" s="1">
-        <f>AVERAGE(G11,M11,S11)</f>
-        <v>38.546666666666667</v>
-      </c>
-      <c r="AA11" s="1">
-        <f>AVERAGE(H11,N11,T11)-Z11</f>
-        <v>56.856666666666655</v>
+      <c r="Z12" s="3">
+        <f>AVERAGE(G12,M12,S12)</f>
+        <v>1.4933333333333334</v>
+      </c>
+      <c r="AA12" s="3">
+        <f>AVERAGE(H12,N12,T12)-Z12</f>
+        <v>2.1466666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
+    <row r="13" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>125</v>
-      </c>
-      <c r="B14" s="2">
-        <f>3*1000/A14</f>
-        <v>24</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2.15</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3.48</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1.67</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="M14" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="N14" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="O14" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0.39</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>1.73</v>
-      </c>
-      <c r="R14" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="S14" s="1">
-        <v>1.36</v>
-      </c>
-      <c r="T14" s="1">
-        <v>2.83</v>
-      </c>
-      <c r="V14" s="1">
-        <f>W14-AVERAGE(C14,I14,O14)</f>
-        <v>0.31000000000000005</v>
-      </c>
-      <c r="W14" s="1">
-        <f>AVERAGE(D14,J14,P14)</f>
-        <v>0.34</v>
-      </c>
-      <c r="X14" s="1">
-        <f>AVERAGE(E14,K14,Q14)-W14</f>
-        <v>0.97666666666666657</v>
-      </c>
-      <c r="Y14" s="1">
-        <f>Z14-AVERAGE(F14,L14,R14)</f>
-        <v>1.3533333333333335</v>
-      </c>
-      <c r="Z14" s="1">
-        <f>AVERAGE(G14,M14,S14)</f>
-        <v>1.8033333333333335</v>
-      </c>
-      <c r="AA14" s="1">
-        <f>AVERAGE(H14,N14,T14)-Z14</f>
-        <v>1.8566666666666667</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove unnecessary decimal point from x axis labels
</commit_message>
<xml_diff>
--- a/evaluation/data/plot.xlsx
+++ b/evaluation/data/plot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/dev/cl/move-op/evaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825C7E1E-7AAF-4B44-891D-A26F9F06FBC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EAE5C6-415D-2348-A8B7-7DFED538ABF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30420" yWindow="-3720" windowWidth="22380" windowHeight="21600" xr2:uid="{0A30AF39-E39C-7545-8255-958495C45241}"/>
+    <workbookView xWindow="52800" yWindow="-9480" windowWidth="24000" windowHeight="38400" xr2:uid="{0A30AF39-E39C-7545-8255-958495C45241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>us-west-1</t>
   </si>
@@ -74,6 +76,39 @@
   <si>
     <t>pos-error</t>
   </si>
+  <si>
+    <t>ap_southeast_1</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>total ops/sec</t>
+  </si>
+  <si>
+    <t>generated ops/sec</t>
+  </si>
+  <si>
+    <t>RTT min</t>
+  </si>
+  <si>
+    <t>RTT median</t>
+  </si>
+  <si>
+    <t>RTT p95</t>
+  </si>
+  <si>
+    <t>Leader mode</t>
+  </si>
+  <si>
+    <t>CRDT mode</t>
+  </si>
+  <si>
+    <t>eu_west_1</t>
+  </si>
+  <si>
+    <t>asymptote</t>
+  </si>
 </sst>
 </file>
 
@@ -82,8 +117,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,11 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -305,10 +349,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$14</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
@@ -341,10 +385,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$4:$Z$14</c:f>
+              <c:f>Sheet1!$Z$4:$Z$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.14333333333333334</c:v>
                 </c:pt>
@@ -416,7 +460,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -645,10 +689,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$X$4:$X$14</c:f>
+                <c:f>Sheet1!$X$4:$X$12</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="11"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>2.6666666666666658E-2</c:v>
                   </c:pt>
@@ -681,10 +725,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$V$4:$V$14</c:f>
+                <c:f>Sheet1!$V$4:$V$12</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="11"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>5.6666666666666671E-2</c:v>
                   </c:pt>
@@ -731,10 +775,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$14</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
@@ -767,10 +811,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$4:$W$14</c:f>
+              <c:f>Sheet1!$W$4:$W$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
@@ -860,7 +904,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -999,6 +1043,1558 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Median RTT eu_west_1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$H$49:$H$61</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>7.00000000000216E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.0000000000002274E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.0000000000002274E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.48999999999998067</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9.0000000000003411E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.0000000000002274E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.0699999999999932</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.84000000000000341</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.9999999999993179E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>25.860000000000014</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>25.690000000000055</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>40.970000000000027</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>35.759999999999991</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$49:$G$61</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>0.84999999999999432</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.0000000000012506E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.0099999999999909</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.0000000000002274E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.9999999999994316E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.0000000000012506E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.49000000000000909</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>195.04</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>389.55999999999995</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>133.68999999999994</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>406.38</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>199.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>399.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>999.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1999.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3999.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9999.32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13963.49</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14346.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13931.28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14184.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$49:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>144.88999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145.52000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>141.66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>144.72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>354.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>697.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>721.16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>705.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C605-9A4F-8D45-936A53BF8651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Median RTT ap_southeast_1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$O$49:$O$61</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>4.9999999999982947E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0000000000001137E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.67000000000001592</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3.0000000000001137E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.66999999999998749</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.0000000000010232E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.3099999999999739</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.0000000000011369E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.9999999999993179E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.48000000000001819</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>31.549999999999955</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>46.629999999999995</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>38.379999999999995</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$N$49:$N$61</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>6.9999999999993179E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.9999999999984084E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.9999999999984084E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.0000000000002274E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9.0000000000003411E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.0000000000011369E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.10000000000002274</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.0000000000011369E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.0000000000002274E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.6299999999999955</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>455.13000000000005</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>430.65</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>520.9</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>199.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>399.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>999.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1999.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3999.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9999.32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13963.49</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14346.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13931.28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14184.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$49:$L$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>173.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>173.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>173.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>173.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>173.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>174.28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>177.79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>695.69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>715.64</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>704.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C605-9A4F-8D45-936A53BF8651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CRDT mode</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>214.29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299.96999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>428.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>499.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>599.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>602.03</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$4:$W$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3333333333333337E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3333333333333337E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3333333333333337E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3333333333333337E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C605-9A4F-8D45-936A53BF8651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1473361872"/>
+        <c:axId val="1473363504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1473361872"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Move operations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1473363504"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1473363504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+          <c:min val="1.0000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time to apply operation (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1473361872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1073,6 +2669,248 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08F4BD3F-BAD5-494C-966C-B4C6F803B7E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35222039-7569-CB45-A654-BB033F710C68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638300" y="15354300"/>
+          <a:ext cx="1866900" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>CRDT local operations</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93F696D7-757A-9F4D-8258-73FD2E055876}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1003300" y="12890500"/>
+          <a:ext cx="2590800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Singapore to leader in California</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07006533-2009-B240-9893-C7511EE094DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="13423900"/>
+          <a:ext cx="2870200" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Ireland to leader in California</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1375,10 +3213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FD8EE4-C80E-7B4A-A3CF-4A016730C7B3}">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,6 +3244,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -2306,8 +4147,15 @@
       </c>
     </row>
     <row r="13" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2">
+        <v>603</v>
+      </c>
+      <c r="W13" s="1">
+        <v>1200</v>
+      </c>
     </row>
     <row r="14" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -2317,6 +4165,685 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="J47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" t="s">
+        <v>20</v>
+      </c>
+      <c r="N48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>100000</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>144.04</v>
+      </c>
+      <c r="E49">
+        <v>144.88999999999999</v>
+      </c>
+      <c r="F49">
+        <v>144.96</v>
+      </c>
+      <c r="G49">
+        <f>E49-D49</f>
+        <v>0.84999999999999432</v>
+      </c>
+      <c r="H49">
+        <f>F49-E49</f>
+        <v>7.00000000000216E-2</v>
+      </c>
+      <c r="J49">
+        <v>10</v>
+      </c>
+      <c r="K49">
+        <v>173.52</v>
+      </c>
+      <c r="L49">
+        <v>173.59</v>
+      </c>
+      <c r="M49">
+        <v>173.64</v>
+      </c>
+      <c r="N49">
+        <f>L49-K49</f>
+        <v>6.9999999999993179E-2</v>
+      </c>
+      <c r="O49">
+        <f>M49-L49</f>
+        <v>4.9999999999982947E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>50000</v>
+      </c>
+      <c r="B50">
+        <v>40</v>
+      </c>
+      <c r="C50">
+        <v>20</v>
+      </c>
+      <c r="D50">
+        <v>140.47999999999999</v>
+      </c>
+      <c r="E50">
+        <v>140.56</v>
+      </c>
+      <c r="F50">
+        <v>140.62</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50:G61" si="13">E50-D50</f>
+        <v>8.0000000000012506E-2</v>
+      </c>
+      <c r="H50">
+        <f t="shared" ref="H50:H61" si="14">F50-E50</f>
+        <v>6.0000000000002274E-2</v>
+      </c>
+      <c r="J50">
+        <v>20</v>
+      </c>
+      <c r="K50">
+        <v>173.68</v>
+      </c>
+      <c r="L50">
+        <v>173.76</v>
+      </c>
+      <c r="M50">
+        <v>173.79</v>
+      </c>
+      <c r="N50">
+        <f t="shared" ref="N50:N61" si="15">L50-K50</f>
+        <v>7.9999999999984084E-2</v>
+      </c>
+      <c r="O50">
+        <f t="shared" ref="O50:O61" si="16">M50-L50</f>
+        <v>3.0000000000001137E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20000</v>
+      </c>
+      <c r="B51">
+        <v>99.99</v>
+      </c>
+      <c r="C51">
+        <v>50</v>
+      </c>
+      <c r="D51">
+        <v>143.83000000000001</v>
+      </c>
+      <c r="E51">
+        <v>144.84</v>
+      </c>
+      <c r="F51">
+        <v>144.9</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="13"/>
+        <v>1.0099999999999909</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="14"/>
+        <v>6.0000000000002274E-2</v>
+      </c>
+      <c r="J51">
+        <v>50</v>
+      </c>
+      <c r="K51">
+        <v>174.11</v>
+      </c>
+      <c r="L51">
+        <v>174.19</v>
+      </c>
+      <c r="M51">
+        <v>174.86</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="15"/>
+        <v>7.9999999999984084E-2</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="16"/>
+        <v>0.67000000000001592</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>10000</v>
+      </c>
+      <c r="B52">
+        <v>199.99</v>
+      </c>
+      <c r="C52">
+        <v>99.99</v>
+      </c>
+      <c r="D52">
+        <v>145.46</v>
+      </c>
+      <c r="E52">
+        <v>145.52000000000001</v>
+      </c>
+      <c r="F52">
+        <v>146.01</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="13"/>
+        <v>6.0000000000002274E-2</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="14"/>
+        <v>0.48999999999998067</v>
+      </c>
+      <c r="J52">
+        <v>99.99</v>
+      </c>
+      <c r="K52">
+        <v>173.47</v>
+      </c>
+      <c r="L52">
+        <v>173.53</v>
+      </c>
+      <c r="M52">
+        <v>173.56</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="15"/>
+        <v>6.0000000000002274E-2</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="16"/>
+        <v>3.0000000000001137E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5000</v>
+      </c>
+      <c r="B53">
+        <v>399.97</v>
+      </c>
+      <c r="C53">
+        <v>199.99</v>
+      </c>
+      <c r="D53">
+        <v>141.16</v>
+      </c>
+      <c r="E53">
+        <v>141.66</v>
+      </c>
+      <c r="F53">
+        <v>141.75</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="14"/>
+        <v>9.0000000000003411E-2</v>
+      </c>
+      <c r="J53">
+        <v>199.99</v>
+      </c>
+      <c r="K53">
+        <v>173.46</v>
+      </c>
+      <c r="L53">
+        <v>173.55</v>
+      </c>
+      <c r="M53">
+        <v>174.22</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="15"/>
+        <v>9.0000000000003411E-2</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="16"/>
+        <v>0.66999999999998749</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2000</v>
+      </c>
+      <c r="B54">
+        <v>999.93</v>
+      </c>
+      <c r="C54">
+        <v>499.97</v>
+      </c>
+      <c r="D54">
+        <v>141.21</v>
+      </c>
+      <c r="E54">
+        <v>141.71</v>
+      </c>
+      <c r="F54">
+        <v>141.77000000000001</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="14"/>
+        <v>6.0000000000002274E-2</v>
+      </c>
+      <c r="J54">
+        <v>499.97</v>
+      </c>
+      <c r="K54">
+        <v>173.01</v>
+      </c>
+      <c r="L54">
+        <v>173.06</v>
+      </c>
+      <c r="M54">
+        <v>173.08</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="15"/>
+        <v>5.0000000000011369E-2</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="16"/>
+        <v>2.0000000000010232E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1000</v>
+      </c>
+      <c r="B55">
+        <v>1999.8</v>
+      </c>
+      <c r="C55">
+        <v>999.9</v>
+      </c>
+      <c r="D55">
+        <v>144.62</v>
+      </c>
+      <c r="E55">
+        <v>144.72</v>
+      </c>
+      <c r="F55">
+        <v>146.79</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="13"/>
+        <v>9.9999999999994316E-2</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="14"/>
+        <v>2.0699999999999932</v>
+      </c>
+      <c r="J55">
+        <v>999.94</v>
+      </c>
+      <c r="K55">
+        <v>173.73</v>
+      </c>
+      <c r="L55">
+        <v>173.83</v>
+      </c>
+      <c r="M55">
+        <v>178.14</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="15"/>
+        <v>0.10000000000002274</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="16"/>
+        <v>4.3099999999999739</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>500</v>
+      </c>
+      <c r="B56">
+        <v>3999.81</v>
+      </c>
+      <c r="C56">
+        <v>1999.87</v>
+      </c>
+      <c r="D56">
+        <v>144.76</v>
+      </c>
+      <c r="E56">
+        <v>144.84</v>
+      </c>
+      <c r="F56">
+        <v>145.68</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="13"/>
+        <v>8.0000000000012506E-2</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="14"/>
+        <v>0.84000000000000341</v>
+      </c>
+      <c r="J56">
+        <v>1999.86</v>
+      </c>
+      <c r="K56">
+        <v>173.73</v>
+      </c>
+      <c r="L56">
+        <v>173.78</v>
+      </c>
+      <c r="M56">
+        <v>173.83</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="15"/>
+        <v>5.0000000000011369E-2</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="16"/>
+        <v>5.0000000000011369E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>200</v>
+      </c>
+      <c r="B57">
+        <v>9999.32</v>
+      </c>
+      <c r="C57">
+        <v>4999.6499999999996</v>
+      </c>
+      <c r="D57">
+        <v>139.51</v>
+      </c>
+      <c r="E57">
+        <v>140</v>
+      </c>
+      <c r="F57">
+        <v>140.07</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="13"/>
+        <v>0.49000000000000909</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="14"/>
+        <v>6.9999999999993179E-2</v>
+      </c>
+      <c r="J57">
+        <v>4999.66</v>
+      </c>
+      <c r="K57">
+        <v>174.22</v>
+      </c>
+      <c r="L57">
+        <v>174.28</v>
+      </c>
+      <c r="M57">
+        <v>174.35</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="15"/>
+        <v>6.0000000000002274E-2</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="16"/>
+        <v>6.9999999999993179E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>50</v>
+      </c>
+      <c r="B58">
+        <v>13963.49</v>
+      </c>
+      <c r="C58">
+        <v>13942.23</v>
+      </c>
+      <c r="D58">
+        <v>159.6</v>
+      </c>
+      <c r="E58">
+        <v>354.64</v>
+      </c>
+      <c r="F58">
+        <v>380.5</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="13"/>
+        <v>195.04</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="14"/>
+        <v>25.860000000000014</v>
+      </c>
+      <c r="J58">
+        <v>20</v>
+      </c>
+      <c r="K58">
+        <v>173.16</v>
+      </c>
+      <c r="L58">
+        <v>177.79</v>
+      </c>
+      <c r="M58">
+        <v>178.27</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="15"/>
+        <v>4.6299999999999955</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="16"/>
+        <v>0.48000000000001819</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>100</v>
+      </c>
+      <c r="B59">
+        <v>14346.52</v>
+      </c>
+      <c r="C59">
+        <v>7249.81</v>
+      </c>
+      <c r="D59">
+        <v>307.86</v>
+      </c>
+      <c r="E59">
+        <v>697.42</v>
+      </c>
+      <c r="F59">
+        <v>723.11</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="13"/>
+        <v>389.55999999999995</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="14"/>
+        <v>25.690000000000055</v>
+      </c>
+      <c r="J59">
+        <v>7093.33</v>
+      </c>
+      <c r="K59">
+        <v>240.56</v>
+      </c>
+      <c r="L59">
+        <v>695.69</v>
+      </c>
+      <c r="M59">
+        <v>727.24</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="15"/>
+        <v>455.13000000000005</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="16"/>
+        <v>31.549999999999955</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>13931.28</v>
+      </c>
+      <c r="C60">
+        <v>6949.35</v>
+      </c>
+      <c r="D60">
+        <v>587.47</v>
+      </c>
+      <c r="E60">
+        <v>721.16</v>
+      </c>
+      <c r="F60">
+        <v>762.13</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="13"/>
+        <v>133.68999999999994</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="14"/>
+        <v>40.970000000000027</v>
+      </c>
+      <c r="J60">
+        <v>6980.84</v>
+      </c>
+      <c r="K60">
+        <v>284.99</v>
+      </c>
+      <c r="L60">
+        <v>715.64</v>
+      </c>
+      <c r="M60">
+        <v>762.27</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="15"/>
+        <v>430.65</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="16"/>
+        <v>46.629999999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>14184.97</v>
+      </c>
+      <c r="C61">
+        <v>7175.63</v>
+      </c>
+      <c r="D61">
+        <v>299.01</v>
+      </c>
+      <c r="E61">
+        <v>705.39</v>
+      </c>
+      <c r="F61">
+        <v>741.15</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="13"/>
+        <v>406.38</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="14"/>
+        <v>35.759999999999991</v>
+      </c>
+      <c r="J61">
+        <v>7004.61</v>
+      </c>
+      <c r="K61">
+        <v>183.6</v>
+      </c>
+      <c r="L61">
+        <v>704.5</v>
+      </c>
+      <c r="M61">
+        <v>742.88</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="15"/>
+        <v>520.9</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="16"/>
+        <v>38.379999999999995</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update fig. 5 to include remote operations and remove asymptote
</commit_message>
<xml_diff>
--- a/evaluation/data/plot.xlsx
+++ b/evaluation/data/plot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/dev/cl/move-op/evaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EAE5C6-415D-2348-A8B7-7DFED538ABF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FF5EF1-CE02-9D4F-ADD5-648377A9AAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52800" yWindow="-9480" windowWidth="24000" windowHeight="38400" xr2:uid="{0A30AF39-E39C-7545-8255-958495C45241}"/>
+    <workbookView xWindow="52800" yWindow="-10120" windowWidth="24000" windowHeight="38400" xr2:uid="{0A30AF39-E39C-7545-8255-958495C45241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1609,7 +1609,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>CRDT mode</c:v>
+            <c:v>CRDT local operations</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1657,10 +1657,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
@@ -1687,19 +1687,16 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>602.03</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0">
-                  <c:v>603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$4:$W$13</c:f>
+              <c:f>Sheet1!$W$4:$W$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
@@ -1726,9 +1723,6 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5.000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>1200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,6 +1731,115 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C605-9A4F-8D45-936A53BF8651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>CRDT remote operations</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>214.29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299.96999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>428.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>499.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>599.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>602.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Z$4:$Z$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.14333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8933333333333332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0233333333333332</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3433333333333335</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4933333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-32C9-3D43-8192-905759682BCE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2710,15 +2813,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2733,7 +2836,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1638300" y="15354300"/>
+          <a:off x="1651000" y="15824200"/>
           <a:ext cx="1866900" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2907,6 +3010,74 @@
               </a:solidFill>
             </a:rPr>
             <a:t>Ireland to leader in California</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0984BD09-F8CB-AC48-9940-75E3E5E0BC5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="14592300"/>
+          <a:ext cx="2171700" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>CRDT remote operations</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3216,7 +3387,7 @@
   <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>